<commit_message>
fixed typo, TS,TC numbers, romoved the step numbers
</commit_message>
<xml_diff>
--- a/Costco-Regression tests.xlsx
+++ b/Costco-Regression tests.xlsx
@@ -58,21 +58,21 @@
     <t>Status</t>
   </si>
   <si>
+    <t>TS001</t>
+  </si>
+  <si>
+    <t>Home page functions</t>
+  </si>
+  <si>
     <t>TC001</t>
   </si>
   <si>
-    <t>Home page functions</t>
-  </si>
-  <si>
-    <t>TS001</t>
-  </si>
-  <si>
     <t xml:space="preserve">User should see diffrent drop down when hower through the menu bar </t>
   </si>
   <si>
-    <t>1.When at the home page
-2.And hower over to "shop" button
-3,And verify that dropdown are displayed. 4. And hower over to "grocery". 5. Then verify that dropdown is changed
+    <t>When at the home page
+And hower over to "shop" button
+And verify that shops dropdown are displayed.  And hower over to "grocery".  Then verify that dropdown is changed
 .</t>
   </si>
   <si>
@@ -85,307 +85,307 @@
     <t>pass</t>
   </si>
   <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>Hero carousel section should slide automaticly</t>
+  </si>
+  <si>
+    <t>When at the home page
+And move to the hero arousel section. And wait for 5 seconds. And verify that slide is changed.  And waite for another 5 seconds. Then verify that slide is changed again</t>
+  </si>
+  <si>
+    <t>hero carousel should changed automaticly evry 5 seconds</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>User should should be able to change the Hero carousel slides manually</t>
+  </si>
+  <si>
+    <t>When at the home page
+And move to the hero arousel section. And click the next arrow button. And verify that slide is changed. And click the prve arrow button. Then verify that slide is changed back</t>
+  </si>
+  <si>
+    <t>hero carousel should be alble changed manually</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>User should get email offers when enter the email at "Get Email Offers" at footer section</t>
+  </si>
+  <si>
+    <t>When at the home page
+And move to "Get Email Offers" at footer section.  And enter an email.  And click "Go". Then verify that the message "Thank you for signing up for our email offers." is displayed.</t>
+  </si>
+  <si>
+    <t>user should be able to get emails offer by giving email</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Social media links should open new page when its click</t>
+  </si>
+  <si>
+    <t>When at the home page
+And move to "Follow Us" at footer section. And click the facebook link. And verify that facebook page is opend. And back to the "Follow Us" section, click the instagram link. Then verify that instagram page is opend</t>
+  </si>
+  <si>
+    <t>social media links should opend in new page</t>
+  </si>
+  <si>
     <t>TS002</t>
   </si>
   <si>
-    <t>Hero carousel section should slide automaticly</t>
-  </si>
-  <si>
-    <t>1. When at the home page
-2.And move to the hero arousel section . 3. And wait for 5 seconds. Then verify that slide is changed. 4. And waite for another 5 seconds. 5.Then verify that slide is changed again</t>
-  </si>
-  <si>
-    <t>hero carousel should changed evry 5 seconds</t>
+    <t>Product page functions</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>Product image, name, model, price, and features should properly displayed</t>
+  </si>
+  <si>
+    <t>When at the home page
+And click an item to be at product page. Then verify that product image, name, model, price and features are displayed</t>
+  </si>
+  <si>
+    <t>bacis necessary info should all displayed</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product page should have following 4 section to click and see: "product details", "sepcifications", "shipping&amp;returns", "reviews" </t>
+  </si>
+  <si>
+    <t>When at the product page
+And click "sepcifications".
+And verify that product details changed to sepecification. And click the "shipping&amp;returns".  And verify that content is changed again. And click the "reviews". Then verify that the content is changed to reviews
+.</t>
+  </si>
+  <si>
+    <t>user should be able to check all the information about the product</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>Floating product info&amp;add to cart section should displayed while scrolling trhough the product page</t>
+  </si>
+  <si>
+    <t>When at the product page
+And scroll to the bottom
+Then verify that small prodcut section is always displayed
+.</t>
+  </si>
+  <si>
+    <t>small product section shouldbe seen when scrolling</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>User should be able to "share", or "print" the product page</t>
+  </si>
+  <si>
+    <t>When at the product page
+And click the "share" link at mid setction
+And verify that all tree social media icon links are displayed. And click the "print" link. Then verify that broswser print pop up is displayed.</t>
+  </si>
+  <si>
+    <t>product page should be shareable and printable</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>User should be able to increment and decrement the quantity of the product</t>
+  </si>
+  <si>
+    <t>When at the product page
+And click increment button at product quantity field.
+And verify that number is incremented. And click decrement buttom. Then verify that the number is decremented.</t>
+  </si>
+  <si>
+    <t>product quantity should be changeable at peroduct page</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>"ErrorQuantity" messeage should be display if user click decrement button when quantity is 1</t>
+  </si>
+  <si>
+    <t>When at the product page
+And click the decrement button. Then verify that  the message " ErrorQuantity must be 1 or more to add to cart." is displayed</t>
+  </si>
+  <si>
+    <t>product quantity should be at leats 1 to add to cart</t>
   </si>
   <si>
     <t>TS003</t>
   </si>
   <si>
-    <t>User should should be able to change the Hero carousel slides manually</t>
-  </si>
-  <si>
-    <t>1. When at the home page
-2.And move to the hero arousel section . 3. And click the next arrow button. Then verify that slide is changed. 4. And click the prve arrow button. 5.Then verify that slide is changed back</t>
-  </si>
-  <si>
-    <t>hero carousel should be alble changed manually</t>
+    <t>Shopping cart page functions</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>Product small image, name, model, price, and shippinng&amp;pickup options should be displayed</t>
+  </si>
+  <si>
+    <t>When at the home page
+And click an item to be at product page. And click "add to cart". And click "view Cart". Then verify that product small image, name, model, price, and shippinng&amp;pickup options should be displayed</t>
+  </si>
+  <si>
+    <t>bacis necessary info should all displayed at shoopping cart page</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>User should be able to remove the item from shopping cart</t>
+  </si>
+  <si>
+    <t>When added item to the cart
+And go to the shopping cart
+And click the remove button in Cart item. Then verify that shopping cart is empty, messeage is displayed.</t>
+  </si>
+  <si>
+    <t>product should be removeable at shopping cart</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>User should be able to save the item for later from shopping cart</t>
+  </si>
+  <si>
+    <t>When added item to the cart
+And go the the shopping cart
+And click the "Save for later" button in Cart item. Then verify that item is moved from cart to "Saved for later"</t>
+  </si>
+  <si>
+    <t>product should be moveable to "save for later" from "cart"</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>User should be add item back to cart from saved for later</t>
+  </si>
+  <si>
+    <t>When added item to the cart
+And go the the shopping cart
+And click the "Save for later" button in Cart item. And click "move to cart" buttom. Then verify that item is added back to the cart</t>
+  </si>
+  <si>
+    <t>items should be moveable to "cart" from "save for later</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t>User should be able to select a Warehouse from pick up option in Cart item</t>
+  </si>
+  <si>
+    <t>When added item to the cart
+And go to the shopping cart.
+3, And click the "Select a Warehouse" button in Cart item. 4. Then verify that "Find a Warehouse" is opend with selection, search bar and map.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pick up location should be selectable in shopping cart </t>
+  </si>
+  <si>
+    <t>TC017</t>
+  </si>
+  <si>
+    <t>"Delivery Details" pop up should be displayed with message contenet when its user click</t>
+  </si>
+  <si>
+    <t>When added item to the cart
+And go to the shopping cart..
+And click the "Delivery Details" in Cart item. Then verify that pop up is displayed with masseage content</t>
+  </si>
+  <si>
+    <t>user should be able to see "Delivery Details" pop up when click it</t>
   </si>
   <si>
     <t>TS004</t>
   </si>
   <si>
-    <t>User should get email offers when enter the email at "Get Email Offers" at footer section</t>
-  </si>
-  <si>
-    <t>1. When at the home page
-2.And move to "Get Email Offers" at footer section . 3. And enter an email. 3.And click "Go". 4.Then verify that the message "Thank you for signing up for our email offers." is displayed.</t>
-  </si>
-  <si>
-    <t>user should be able to get emails offer by giving email</t>
-  </si>
-  <si>
-    <t>TS005</t>
-  </si>
-  <si>
-    <t>Social media links should open new page when its click</t>
-  </si>
-  <si>
-    <t>1. When at the home page
-2.And move to "Follow Us" at footer section . 3. And click the facebook link. 3. Then verify that facebook page is opend. 4. And back to the "Follow Us" section, click the instagram link. 5.Then verify that instagram page is opend</t>
-  </si>
-  <si>
-    <t>social media links should opend in new page</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>Product page functions</t>
-  </si>
-  <si>
-    <t>TS006</t>
-  </si>
-  <si>
-    <t>Product image, name, model, price, and features should properly displayed</t>
-  </si>
-  <si>
-    <t>1. When at the home page
-2.And click an item to be at product page. 3. Then verify that product image, name, model, price and features are displayed</t>
-  </si>
-  <si>
-    <t>bacis necessary info should all displayed</t>
-  </si>
-  <si>
-    <t>TS007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product page should have following 4 section to click and see: "product details", "sepcifications", "shipping&amp;returns", "reviews" </t>
-  </si>
-  <si>
-    <t>1.When at the product page
-2.And click "sepcifications".
-3, And verify that product details changed to sepecification. 4.And click the "shipping&amp;returns". 5. And verify that content is changed again. 6. And click the "reviews". 7.Then verify that the content is changed to reviews
-.</t>
-  </si>
-  <si>
-    <t>user should be able to check all the information about the product</t>
-  </si>
-  <si>
-    <t>TS008</t>
-  </si>
-  <si>
-    <t>Floating product info&amp;add to cart section should displayed while crolling trhough the product page</t>
-  </si>
-  <si>
-    <t>1.When at the product page
-2.And scroll to the button
-3, Then verify that small prodcut section is always displayed
-.</t>
-  </si>
-  <si>
-    <t>small product section shouldbe seen when scrolling</t>
-  </si>
-  <si>
-    <t>TS009</t>
-  </si>
-  <si>
-    <t>User should be able to "share", or "print" the product page</t>
-  </si>
-  <si>
-    <t>1.When at the product page
-2.And click the "share" link at mid setction
-3, And verify that all tree social media icon links are displayed. 4.And click the "print" link. 5.Then verify that broswser print pop up is displayed.</t>
-  </si>
-  <si>
-    <t>product page should be shareable and printable</t>
-  </si>
-  <si>
-    <t>TS010</t>
-  </si>
-  <si>
-    <t>User should be able to increment and decrement the quantity of the product</t>
-  </si>
-  <si>
-    <t>1.When at the product page
-2.And click increment button at product quantity field.
-3, And verify that number is incremented 2. 4.And click decrement buttom 5.Then verify that the number is decremented.</t>
-  </si>
-  <si>
-    <t>product quantity should be changeable at peroduct page</t>
-  </si>
-  <si>
-    <t>TS011</t>
-  </si>
-  <si>
-    <t>"ErrorQuantity" messeage should be display if user click decrement button when quantity is 1</t>
-  </si>
-  <si>
-    <t>1.When at the product page
-2.And click the decrement button. 3.Then verify that  the message " ErrorQuantity must be 1 or more to add to cart." is displayed</t>
-  </si>
-  <si>
-    <t>product quantity should be at leats 1 to add to cart</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>Shopping cart functions</t>
-  </si>
-  <si>
-    <t>TS012</t>
-  </si>
-  <si>
-    <t>Product small image, name, model, price, and shippinng&amp;pickup options should be displayed</t>
-  </si>
-  <si>
-    <t>1. When at the home page
-2.And click an item to be at product page. 3.And click "add to cart". 4, And click "view Cart". 5. Then verify that product small image, name, model, price, and shippinng&amp;pickup options should be displayed</t>
-  </si>
-  <si>
-    <t>bacis necessary info should all displayed at shoopping cart page</t>
-  </si>
-  <si>
-    <t>TS013</t>
-  </si>
-  <si>
-    <t>User should be able to remove the item from shopping cart</t>
-  </si>
-  <si>
-    <t>1.When added item to the cart
-2.And go to the shopping cart
-3, And click the remove button in Cart item. 4.Then verify that shopping cart is empty, messeage is displayed.</t>
-  </si>
-  <si>
-    <t>product should be removeable at shopping cart</t>
-  </si>
-  <si>
-    <t>TS014</t>
-  </si>
-  <si>
-    <t>User should be able to save the item for later from shopping cart</t>
-  </si>
-  <si>
-    <t>1.When added item to the cart
-2.And go the the shopping cart
-3, And click the "Save for later" button in Cart item. 4. Then verify that item is moved from cart to "Saved for later"</t>
-  </si>
-  <si>
-    <t>product should be moveable to "save for later" from "cart"</t>
-  </si>
-  <si>
-    <t>TS015</t>
-  </si>
-  <si>
-    <t>User should be add item back to cart from saved for later</t>
-  </si>
-  <si>
-    <t>1.When added item to the cart
-2.And go the the shopping cart
-3, And click the "Save for later" button in Cart item. 4.And click "move to cart" buttom. 5.verify that item is added back to the cart</t>
-  </si>
-  <si>
-    <t>items should be moveable to "cart" from "save for later</t>
-  </si>
-  <si>
-    <t>TS016</t>
-  </si>
-  <si>
-    <t>User should be able to select a Warehouse for pick up option in Cart item</t>
-  </si>
-  <si>
-    <t>1.When at the product page
-2.And click increment button at product quantity field.
-3, And click the "Select a Warehouse" button in Cart item. 4. Then verify that "Find a Warehouse" is opend with selection, search bar and map.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pick up location should be selectable in shopping cart </t>
-  </si>
-  <si>
-    <t>TS017</t>
-  </si>
-  <si>
-    <t>"Delivery Details" pop up should be displayed with message contenet when its user click</t>
-  </si>
-  <si>
-    <t>1.When at the product page
-2.And click increment button at product quantity field.
-3, And click the "Delivery Details" in Cart item. 4.Then verify that pop up is displayed with masseage content</t>
-  </si>
-  <si>
-    <t>user should be able to see "Delivery Details" pop up when click it</t>
-  </si>
-  <si>
-    <t>TC004</t>
-  </si>
-  <si>
     <t>Result page fonctions</t>
   </si>
   <si>
-    <t>TS018</t>
+    <t>TC018</t>
   </si>
   <si>
     <t>"Filter Results" should have following 4 options: "category", "Price", "Brand", "Features"</t>
   </si>
   <si>
-    <t>1. When at the home page
-2.And search for "coffees" at search bar and enter. 3 And verify that all 4 filter options are displayed unser"Filter Results"</t>
+    <t>When at the home page
+And search for "coffees" at search bar and enter. And verify that all 4 filter options are displayed unser"Filter Results"</t>
   </si>
   <si>
     <t xml:space="preserve">user should be able to filtter the result </t>
   </si>
   <si>
-    <t>TS019</t>
+    <t>TC019</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to view the resullts by "blocks" or "list" way by changeging grid-view </t>
   </si>
   <si>
-    <t>1.When at result page sreached for "coffees"
-2.And click the "List view" button.
-3, And verify that results veiew is changed to list. 4.And click the "block view" button. 5.Then verify that results view is changed to block</t>
+    <t>When at result page sreached for "coffees"
+And click the "List view" button.
+And verify that results veiew is changed to list. And click the "block view" button. Then verify that results view is changed to block</t>
   </si>
   <si>
     <t>product should be removeable at shopping cart page</t>
   </si>
   <si>
-    <t>TS020</t>
+    <t>TC020</t>
   </si>
   <si>
     <t>User should be able to back to the top when at the bottom of results page</t>
   </si>
   <si>
-    <t>1.When at result page sreached for "coffees"
-2.And scroll to the end of results section
-3, And click the "back to top" buttom. 4.Then verify that page is scroll back to the top</t>
+    <t>When at result page sreached for "coffees"
+And scroll to the end of results section
+And click the "back to top" buttom. Then verify that page is scroll back to the top</t>
   </si>
   <si>
     <t>user back to the top of result page by one click</t>
   </si>
   <si>
-    <t>TS021</t>
+    <t>TC021</t>
   </si>
   <si>
     <t>User should be able to sort the result by "price(low to high)"</t>
   </si>
   <si>
-    <t>1.When at result page sreached for "coffees"
-2.And click the "sort by" drop down in search results
-3, And click "price(low to high)" option. 4.Then verify that results is sorted by price low to high</t>
+    <t>When at result page sreached for "coffees"
+And click the "sort by" drop down in search results
+And click "price(low to high)" option. Then verify that results is sorted by price low to high</t>
   </si>
   <si>
     <t>result should be sortable by price</t>
   </si>
   <si>
-    <t>TS022</t>
+    <t>TC022</t>
   </si>
   <si>
     <t>User should be able to filter the result by "price" range</t>
   </si>
   <si>
-    <t>1.When at result page sreached for "coffees"
-2.And move to the "price" section is "Filter rsults"
-3, And click "$0 ~ $25" chckbox . 4.Then verify that results is filtered.</t>
+    <t>When at result page sreached for "coffees"
+And move to the "price" section in "Filter rsults"
+And click "$0 ~ $25" checkbox. Then verify that results is filtered.</t>
   </si>
   <si>
     <t>result should be filtterable by price</t>
@@ -405,17 +405,14 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
-      <color theme="1"/>
       <name val="Averta"/>
     </font>
   </fonts>
@@ -494,6 +491,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -501,9 +501,6 @@
     </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,7 +719,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="17.86"/>
-    <col customWidth="1" min="5" max="5" width="29.14"/>
+    <col customWidth="1" min="5" max="5" width="30.71"/>
+    <col customWidth="1" min="6" max="6" width="22.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -821,35 +819,35 @@
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -858,76 +856,76 @@
       <c r="F8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="9" t="s">
+      <c r="G10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="9" t="s">
+      <c r="G11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -935,53 +933,53 @@
       <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="G12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="G13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="7" t="s">
         <v>49</v>
       </c>
@@ -991,79 +989,79 @@
       <c r="E14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="9" t="s">
+      <c r="G14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="8" t="s">
         <v>54</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="9" t="s">
+      <c r="G15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="9" t="s">
+      <c r="G16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="9" t="s">
+      <c r="G17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1077,91 +1075,91 @@
       <c r="C18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="9" t="s">
+      <c r="G18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="9" t="s">
+      <c r="G19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="9" t="s">
+      <c r="G20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="9" t="s">
+      <c r="G21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="7" t="s">
         <v>83</v>
       </c>
@@ -1171,35 +1169,35 @@
       <c r="E22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="9" t="s">
+      <c r="G22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="8" t="s">
         <v>88</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="9" t="s">
+      <c r="G23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1207,113 +1205,113 @@
       <c r="A24" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>92</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="8" t="s">
         <v>94</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="9" t="s">
+      <c r="G24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="8" t="s">
         <v>98</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="9" t="s">
+      <c r="G25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>102</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" s="9" t="s">
+      <c r="G26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="8" t="s">
         <v>106</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="9" t="s">
+      <c r="G27" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="8" t="s">
         <v>110</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" s="9" t="s">
+      <c r="G28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="10" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>